<commit_message>
Modified the code to output the codebook in markdown format
</commit_message>
<xml_diff>
--- a/Farm.xlsx
+++ b/Farm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/belendia/Documents/Projects/PythonProj/Codebook-ODK/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/belendia/Documents/Projects/PythonProj/XLSForm-2-Codebook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C61D727-C113-2649-AC93-A60FCA7FA407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B97353F-4089-4E4B-B9D7-B71AA9979ADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{344615F0-7652-2245-AA89-D5C1186BC530}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" activeTab="2" xr2:uid="{344615F0-7652-2245-AA89-D5C1186BC530}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="204">
   <si>
     <t>text</t>
   </si>
@@ -533,12 +533,6 @@
     <t>jr:choice-name(${farm_code},'${farm_code}')</t>
   </si>
   <si>
-    <t>]Farm Survey</t>
-  </si>
-  <si>
-    <t>ef</t>
-  </si>
-  <si>
     <t>Interviewer 1</t>
   </si>
   <si>
@@ -708,13 +702,25 @@
   </si>
   <si>
     <t>Farm 32</t>
+  </si>
+  <si>
+    <t>public_key</t>
+  </si>
+  <si>
+    <t>Farm Survey</t>
+  </si>
+  <si>
+    <t>ef_2</t>
+  </si>
+  <si>
+    <t>https://kc.kobotoolbox.org/pomi/submission</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -941,6 +947,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -1008,7 +1022,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1017,8 +1031,9 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1157,11 +1172,15 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="20% - Accent3" xfId="3" builtinId="38"/>
     <cellStyle name="40% - Accent3" xfId="4" builtinId="39"/>
     <cellStyle name="Accent2" xfId="2" builtinId="33"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="5" xr:uid="{CBD57AD2-FBDC-3943-AA65-246A28DF0BDA}"/>
     <cellStyle name="Output" xfId="1" builtinId="21"/>
@@ -1478,8 +1497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DCC63E6-B035-0C4D-9290-0BEF76156731}">
   <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2108,7 +2127,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F93DAA9A-B933-464D-838D-0FBBC3F65C25}">
   <dimension ref="A1:D93"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C39" sqref="C39:C70"/>
     </sheetView>
   </sheetViews>
@@ -2241,7 +2260,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D13" s="26">
         <v>1</v>
@@ -2255,7 +2274,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D14" s="26">
         <v>1</v>
@@ -2269,7 +2288,7 @@
         <v>3</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D15" s="26">
         <v>1</v>
@@ -2283,7 +2302,7 @@
         <v>4</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D16" s="26">
         <v>1</v>
@@ -2297,7 +2316,7 @@
         <v>5</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D17" s="26">
         <v>1</v>
@@ -2311,7 +2330,7 @@
         <v>6</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D18" s="26">
         <v>2</v>
@@ -2325,7 +2344,7 @@
         <v>7</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D19" s="26">
         <v>2</v>
@@ -2339,7 +2358,7 @@
         <v>8</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D20" s="26">
         <v>2</v>
@@ -2353,7 +2372,7 @@
         <v>9</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D21" s="26">
         <v>2</v>
@@ -2367,7 +2386,7 @@
         <v>10</v>
       </c>
       <c r="C22" s="23" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D22" s="26">
         <v>2</v>
@@ -2381,7 +2400,7 @@
         <v>11</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D23" s="26">
         <v>3</v>
@@ -2395,7 +2414,7 @@
         <v>12</v>
       </c>
       <c r="C24" s="23" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D24" s="26">
         <v>3</v>
@@ -2409,7 +2428,7 @@
         <v>13</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D25" s="26">
         <v>3</v>
@@ -2423,7 +2442,7 @@
         <v>14</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D26" s="26">
         <v>3</v>
@@ -2437,7 +2456,7 @@
         <v>15</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D27" s="26">
         <v>3</v>
@@ -2451,7 +2470,7 @@
         <v>16</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D28" s="26">
         <v>4</v>
@@ -2465,7 +2484,7 @@
         <v>17</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D29" s="26">
         <v>4</v>
@@ -2479,7 +2498,7 @@
         <v>18</v>
       </c>
       <c r="C30" s="23" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D30" s="26">
         <v>4</v>
@@ -2493,7 +2512,7 @@
         <v>19</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D31" s="26">
         <v>4</v>
@@ -2507,7 +2526,7 @@
         <v>20</v>
       </c>
       <c r="C32" s="23" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D32" s="26">
         <v>4</v>
@@ -2521,7 +2540,7 @@
         <v>21</v>
       </c>
       <c r="C33" s="23" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D33" s="26">
         <v>5</v>
@@ -2535,7 +2554,7 @@
         <v>22</v>
       </c>
       <c r="C34" s="23" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D34" s="26">
         <v>5</v>
@@ -2549,7 +2568,7 @@
         <v>23</v>
       </c>
       <c r="C35" s="23" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D35" s="26">
         <v>5</v>
@@ -2563,7 +2582,7 @@
         <v>24</v>
       </c>
       <c r="C36" s="23" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D36" s="26">
         <v>5</v>
@@ -2577,7 +2596,7 @@
         <v>25</v>
       </c>
       <c r="C37" s="23" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D37" s="26">
         <v>5</v>
@@ -2596,7 +2615,7 @@
         <v>115</v>
       </c>
       <c r="C39" s="23" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D39" s="26">
         <v>1</v>
@@ -2610,7 +2629,7 @@
         <v>1</v>
       </c>
       <c r="C40" s="23" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D40" s="26">
         <v>1</v>
@@ -2624,7 +2643,7 @@
         <v>17</v>
       </c>
       <c r="C41" s="23" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D41" s="26">
         <v>1</v>
@@ -2638,7 +2657,7 @@
         <v>83</v>
       </c>
       <c r="C42" s="23" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D42" s="26">
         <v>1</v>
@@ -2652,7 +2671,7 @@
         <v>39</v>
       </c>
       <c r="C43" s="23" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D43" s="26">
         <v>1</v>
@@ -2666,7 +2685,7 @@
         <v>43</v>
       </c>
       <c r="C44" s="23" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D44" s="26">
         <v>1</v>
@@ -2680,7 +2699,7 @@
         <v>18</v>
       </c>
       <c r="C45" s="23" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D45" s="26">
         <v>1</v>
@@ -2694,7 +2713,7 @@
         <v>33</v>
       </c>
       <c r="C46" s="23" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D46" s="26">
         <v>1</v>
@@ -2708,7 +2727,7 @@
         <v>20</v>
       </c>
       <c r="C47" s="23" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D47" s="26">
         <v>1</v>
@@ -2722,7 +2741,7 @@
         <v>5</v>
       </c>
       <c r="C48" s="23" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D48" s="26">
         <v>1</v>
@@ -2736,7 +2755,7 @@
         <v>37</v>
       </c>
       <c r="C49" s="23" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D49" s="26">
         <v>1</v>
@@ -2750,7 +2769,7 @@
         <v>6</v>
       </c>
       <c r="C50" s="23" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D50" s="26">
         <v>1</v>
@@ -2764,7 +2783,7 @@
         <v>32</v>
       </c>
       <c r="C51" s="23" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D51" s="26">
         <v>1</v>
@@ -2778,7 +2797,7 @@
         <v>7</v>
       </c>
       <c r="C52" s="23" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D52" s="26">
         <v>1</v>
@@ -2792,7 +2811,7 @@
         <v>28</v>
       </c>
       <c r="C53" s="23" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D53" s="26">
         <v>1</v>
@@ -2806,7 +2825,7 @@
         <v>22</v>
       </c>
       <c r="C54" s="23" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D54" s="26">
         <v>1</v>
@@ -2820,7 +2839,7 @@
         <v>19</v>
       </c>
       <c r="C55" s="23" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D55" s="26">
         <v>1</v>
@@ -2834,7 +2853,7 @@
         <v>93</v>
       </c>
       <c r="C56" s="23" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D56" s="26">
         <v>1</v>
@@ -2848,7 +2867,7 @@
         <v>70</v>
       </c>
       <c r="C57" s="23" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D57" s="26">
         <v>1</v>
@@ -2862,7 +2881,7 @@
         <v>103</v>
       </c>
       <c r="C58" s="23" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D58" s="26">
         <v>1</v>
@@ -2876,7 +2895,7 @@
         <v>8</v>
       </c>
       <c r="C59" s="23" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D59" s="26">
         <v>1</v>
@@ -2890,7 +2909,7 @@
         <v>27</v>
       </c>
       <c r="C60" s="23" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D60" s="26">
         <v>1</v>
@@ -2904,7 +2923,7 @@
         <v>48</v>
       </c>
       <c r="C61" s="23" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D61" s="26">
         <v>1</v>
@@ -2918,7 +2937,7 @@
         <v>13</v>
       </c>
       <c r="C62" s="23" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D62" s="26">
         <v>1</v>
@@ -2932,7 +2951,7 @@
         <v>25</v>
       </c>
       <c r="C63" s="23" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D63" s="26">
         <v>1</v>
@@ -2946,7 +2965,7 @@
         <v>36</v>
       </c>
       <c r="C64" s="23" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D64" s="26">
         <v>1</v>
@@ -2960,7 +2979,7 @@
         <v>4</v>
       </c>
       <c r="C65" s="23" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D65" s="26">
         <v>1</v>
@@ -2974,7 +2993,7 @@
         <v>2</v>
       </c>
       <c r="C66" s="23" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D66" s="26">
         <v>1</v>
@@ -2988,7 +3007,7 @@
         <v>3</v>
       </c>
       <c r="C67" s="23" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D67" s="26">
         <v>1</v>
@@ -3002,7 +3021,7 @@
         <v>15</v>
       </c>
       <c r="C68" s="23" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D68" s="26">
         <v>1</v>
@@ -3016,7 +3035,7 @@
         <v>9</v>
       </c>
       <c r="C69" s="23" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D69" s="26">
         <v>1</v>
@@ -3030,7 +3049,7 @@
         <v>62</v>
       </c>
       <c r="C70" s="23" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D70" s="26">
         <v>1</v>
@@ -3266,10 +3285,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A499AFAC-677C-E142-9567-DDAF7EEE2B07}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3277,9 +3296,10 @@
     <col min="1" max="1" width="36.1640625" customWidth="1"/>
     <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="65.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="32" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="32" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="38" t="s">
         <v>85</v>
       </c>
@@ -3298,13 +3318,16 @@
       <c r="F1" s="32" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" s="34" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="G1" s="32" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="34" customFormat="1" ht="226" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="33" t="s">
-        <v>143</v>
+        <v>201</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>144</v>
+        <v>202</v>
       </c>
       <c r="C2" s="34" t="s">
         <v>91</v>
@@ -3312,11 +3335,17 @@
       <c r="D2" s="35" t="s">
         <v>98</v>
       </c>
+      <c r="E2" s="48" t="s">
+        <v>203</v>
+      </c>
       <c r="F2" s="34">
-        <v>20221003</v>
+        <v>20230309</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{F6014BA9-22F6-EA4D-8B5C-A037B7D06ABF}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>